<commit_message>
Inclusão de testes de login e tentativa de upload de arquivo.
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven.xlsx
+++ b/src/test/resources/dataDriven.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karini\git\avaliacaoSambatech\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="1005"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>